<commit_message>
Fix Merge branch 'feature/global-exception-handling' of https://github.com/dennishendriksen/molgenis into feature/global-exception-handling
</commit_message>
<xml_diff>
--- a/molgenis-data-import/src/test/resources/example.xlsx
+++ b/molgenis-data-import/src/test/resources/example.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\molgenis\molgenis-data-import\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -109,13 +114,19 @@
   </si>
   <si>
     <t>parent</t>
+  </si>
+  <si>
+    <t>backend</t>
+  </si>
+  <si>
+    <t>varken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,19 +202,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -217,10 +228,18 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -552,7 +571,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
@@ -692,35 +711,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -742,11 +767,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -850,7 +875,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>